<commit_message>
updated examples and gitignore
</commit_message>
<xml_diff>
--- a/example/data/files_info.xlsx
+++ b/example/data/files_info.xlsx
@@ -513,10 +513,8 @@
       <c r="G2" t="n">
         <v>1</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
+      <c r="H2" t="n">
+        <v>210</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>
@@ -553,10 +551,8 @@
       <c r="G3" t="n">
         <v>1</v>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
+      <c r="H3" t="n">
+        <v>210</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
@@ -593,10 +589,8 @@
       <c r="G4" t="n">
         <v>1</v>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
+      <c r="H4" t="n">
+        <v>210</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -633,10 +627,8 @@
       <c r="G5" t="n">
         <v>1</v>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
+      <c r="H5" t="n">
+        <v>210</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
@@ -673,10 +665,8 @@
       <c r="G6" t="n">
         <v>1</v>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>254</t>
-        </is>
+      <c r="H6" t="n">
+        <v>254</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
@@ -713,10 +703,8 @@
       <c r="G7" t="n">
         <v>1</v>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>254</t>
-        </is>
+      <c r="H7" t="n">
+        <v>254</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
@@ -753,10 +741,8 @@
       <c r="G8" t="n">
         <v>1</v>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>254</t>
-        </is>
+      <c r="H8" t="n">
+        <v>254</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
@@ -793,10 +779,8 @@
       <c r="G9" t="n">
         <v>1</v>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>254</t>
-        </is>
+      <c r="H9" t="n">
+        <v>254</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
@@ -833,10 +817,8 @@
       <c r="G10" t="n">
         <v>1</v>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>254</t>
-        </is>
+      <c r="H10" t="n">
+        <v>254</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>

</xml_diff>